<commit_message>
Committing work that we are doing in TZ
</commit_message>
<xml_diff>
--- a/menuSpreadSheet.xlsx
+++ b/menuSpreadSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="1760" yWindow="1760" windowWidth="23840" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="470">
   <si>
     <t>Text</t>
   </si>
@@ -1508,8 +1508,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="685">
+  <cellStyleXfs count="693">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2199,7 +2207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="685">
+  <cellStyles count="693">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2542,6 +2550,10 @@
     <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2884,6 +2896,10 @@
     <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3222,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I245"/>
+  <dimension ref="A1:I246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F206" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I218" sqref="I218:I245"/>
+    <sheetView tabSelected="1" topLeftCell="G235" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="I246" sqref="I246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -10071,7 +10087,7 @@
         <v>195</v>
       </c>
       <c r="I218" t="str">
-        <f t="shared" ref="I218:I245" si="24">"{" &amp; B218 &amp; "Str, " &amp; C218 &amp;  ", " &amp; D218 &amp; ", " &amp; E218 &amp; ", " &amp; F218 &amp; ", " &amp; G218 &amp; ", " &amp; H218&amp;"},"</f>
+        <f t="shared" ref="I218:I246" si="24">"{" &amp; B218 &amp; "Str, " &amp; C218 &amp;  ", " &amp; D218 &amp; ", " &amp; E218 &amp; ", " &amp; F218 &amp; ", " &amp; G218 &amp; ", " &amp; H218&amp;"},"</f>
         <v>{extrudeRootStr, -1, 1, NULL, 0, Menu::TITLE, &amp;exitExtrude},</v>
       </c>
     </row>
@@ -10109,7 +10125,7 @@
     </row>
     <row r="220" spans="1:9">
       <c r="A220">
-        <f t="shared" ref="A220:A245" si="25">A219+1</f>
+        <f t="shared" ref="A220:A246" si="25">A219+1</f>
         <v>2</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -10722,7 +10738,7 @@
         <v>26</v>
       </c>
       <c r="C239">
-        <f t="shared" ref="C239:C245" si="27">$A$218</f>
+        <f t="shared" ref="C239:C246" si="27">$A$218</f>
         <v>0</v>
       </c>
       <c r="D239">
@@ -10935,6 +10951,37 @@
       <c r="I245" t="str">
         <f t="shared" si="24"/>
         <v>{soakTimeStr, 0, -1, &amp;configuration.profile.soakTime, 0, Menu::DOUBLE, NULL},</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9">
+      <c r="A246">
+        <f t="shared" si="25"/>
+        <v>28</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>-1</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F246">
+        <v>2</v>
+      </c>
+      <c r="G246" t="s">
+        <v>38</v>
+      </c>
+      <c r="H246" t="s">
+        <v>291</v>
+      </c>
+      <c r="I246" t="str">
+        <f t="shared" si="24"/>
+        <v>{spoolerDiskRadiusStr, 0, -1, &amp;configuration.physical.spoolerDiskRadius, 2, Menu::FLOAT, &amp;setOutfeedRPM},</v>
       </c>
     </row>
   </sheetData>
@@ -10952,8 +10999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C148" sqref="C2:C148"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="25" x14ac:dyDescent="0"/>

</xml_diff>